<commit_message>
re-run experiment results and tests for influence/sensitivity experiments
</commit_message>
<xml_diff>
--- a/parameter_files/base/lambdas.xlsx
+++ b/parameter_files/base/lambdas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{DE7AA214-7A52-45FD-B34D-95B35E7A1CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39A0DA2C-2A7D-40F7-AA32-D5EBA5DF0D1A}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{DE7AA214-7A52-45FD-B34D-95B35E7A1CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E4FE022-3C53-422B-B483-80DB70618180}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5AFC58BC-5DA4-4BEE-A195-DB852AED1E19}"/>
   </bookViews>
@@ -726,10 +726,10 @@
   <dimension ref="A1:AI35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -875,7 +875,7 @@
       <c r="B4" s="16"/>
       <c r="H4" s="6"/>
       <c r="W4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>

</xml_diff>

<commit_message>
change parameters (lambdas), add code for comparing
</commit_message>
<xml_diff>
--- a/parameter_files/base/lambdas.xlsx
+++ b/parameter_files/base/lambdas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{DE7AA214-7A52-45FD-B34D-95B35E7A1CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E4FE022-3C53-422B-B483-80DB70618180}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{DE7AA214-7A52-45FD-B34D-95B35E7A1CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20C570CF-934C-428F-9C91-08B284767C40}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5AFC58BC-5DA4-4BEE-A195-DB852AED1E19}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5AFC58BC-5DA4-4BEE-A195-DB852AED1E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -715,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -726,10 +726,10 @@
   <dimension ref="A1:AI35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -861,9 +861,6 @@
       </c>
       <c r="B3" s="16"/>
       <c r="H3" s="6"/>
-      <c r="W3">
-        <v>1</v>
-      </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>

</xml_diff>